<commit_message>
Corretto diagrammi e packages
</commit_message>
<xml_diff>
--- a/Documenti progetto/Diagrammi/MatriceAccessi.xlsx
+++ b/Documenti progetto/Diagrammi/MatriceAccessi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alfredo\Documents\Codice\Java Projects\SecondLifeTech\Documenti progetto\Diagrammi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BA0AEB-388D-4702-A654-CA13DFD9A099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6E40C1-7A0A-406D-A771-5E25981D32E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{5434EAE2-D7D8-43B2-9D75-0F7C7BCB0F51}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5434EAE2-D7D8-43B2-9D75-0F7C7BCB0F51}"/>
   </bookViews>
   <sheets>
     <sheet name="GestioneUtenti" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -295,7 +295,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -401,7 +401,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -543,7 +543,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961D7DE2-08B2-418B-9A49-AFD66138B1B0}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="K6" sqref="A1:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,10 +697,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
@@ -732,10 +732,10 @@
         <v>1</v>
       </c>
       <c r="H5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" s="5">
         <v>0</v>
@@ -767,10 +767,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5">
         <v>0</v>
@@ -1224,7 +1224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CB95E6-C44D-448B-B25E-BD5636143938}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>